<commit_message>
modify id convention for more comprehensibility
</commit_message>
<xml_diff>
--- a/IDSheet.xlsx
+++ b/IDSheet.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Learning\HK2Nam2\Introduction to Game Development\GameDev\GameMario\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C09206B3-5255-46E8-9A80-5AFB9E79C36C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC9706D5-69FE-49E3-BE28-836BAA08FC8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Dynamic Object" sheetId="1" r:id="rId1"/>
+    <sheet name="Static Object" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="36">
   <si>
     <t>Object</t>
   </si>
@@ -115,6 +116,24 @@
   </si>
   <si>
     <t>walking left</t>
+  </si>
+  <si>
+    <t>goomba</t>
+  </si>
+  <si>
+    <t>brick</t>
+  </si>
+  <si>
+    <t>coin</t>
+  </si>
+  <si>
+    <t>cloud</t>
+  </si>
+  <si>
+    <t>walk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">walk </t>
   </si>
 </sst>
 </file>
@@ -441,10 +460,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F55"/>
+  <dimension ref="A1:F62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F58" sqref="F58"/>
+    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A63" sqref="A63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -607,170 +626,170 @@
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C18" t="s">
+        <v>15</v>
+      </c>
       <c r="D18">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C19" t="s">
+        <v>311</v>
+      </c>
+      <c r="E18" t="s">
         <v>15</v>
       </c>
-      <c r="D19">
-        <v>311</v>
-      </c>
-      <c r="E19" t="s">
-        <v>15</v>
-      </c>
-      <c r="F19">
+      <c r="F18">
         <v>310</v>
       </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C20" t="s">
+        <v>16</v>
+      </c>
       <c r="D20">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C22" t="s">
+        <v>401</v>
+      </c>
+      <c r="E20" t="s">
         <v>16</v>
       </c>
-      <c r="D22">
-        <v>401</v>
-      </c>
-      <c r="E22" t="s">
-        <v>16</v>
-      </c>
-      <c r="F22">
+      <c r="F20">
         <v>400</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C21" t="s">
+        <v>17</v>
+      </c>
+      <c r="D21">
+        <v>411</v>
+      </c>
+      <c r="E21" t="s">
+        <v>17</v>
+      </c>
+      <c r="F21">
+        <v>410</v>
       </c>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C23" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D23">
-        <v>411</v>
+        <v>501</v>
       </c>
       <c r="E23" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F23">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C25" t="s">
-        <v>19</v>
-      </c>
-      <c r="D25">
-        <v>501</v>
-      </c>
-      <c r="E25" t="s">
-        <v>19</v>
-      </c>
-      <c r="F25">
         <v>500</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C24" t="s">
+        <v>18</v>
+      </c>
+      <c r="D24">
+        <v>511</v>
+      </c>
+      <c r="E24" t="s">
+        <v>18</v>
+      </c>
+      <c r="F24">
+        <v>510</v>
       </c>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C26" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D26">
-        <v>511</v>
+        <v>601</v>
       </c>
       <c r="E26" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F26">
-        <v>510</v>
-      </c>
-    </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C28" t="s">
-        <v>20</v>
-      </c>
-      <c r="D28">
-        <v>601</v>
-      </c>
-      <c r="E28" t="s">
-        <v>20</v>
-      </c>
-      <c r="F28">
         <v>600</v>
       </c>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C29" t="s">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C27" t="s">
         <v>21</v>
       </c>
-      <c r="D29">
+      <c r="D27">
         <v>611</v>
       </c>
-      <c r="E29" t="s">
+      <c r="E27" t="s">
         <v>21</v>
       </c>
-      <c r="F29">
+      <c r="F27">
         <v>610</v>
       </c>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B32" t="s">
+    <row r="30" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B30" t="s">
         <v>23</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C30" t="s">
         <v>9</v>
       </c>
-      <c r="D32">
-        <v>1001</v>
-      </c>
-      <c r="E32" t="s">
+      <c r="D30">
+        <v>2001</v>
+      </c>
+      <c r="E30" t="s">
         <v>9</v>
       </c>
-      <c r="F32">
-        <v>1000</v>
+      <c r="F30">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C31" t="s">
+        <v>24</v>
+      </c>
+      <c r="D31">
+        <v>2011</v>
+      </c>
+      <c r="E31" t="s">
+        <v>8</v>
+      </c>
+      <c r="F31">
+        <v>2010</v>
       </c>
     </row>
     <row r="33" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C33" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D33">
-        <v>1011</v>
+        <v>2101</v>
       </c>
       <c r="E33" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="F33">
-        <v>1010</v>
+        <v>2100</v>
+      </c>
+    </row>
+    <row r="34" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="D34">
+        <v>2102</v>
       </c>
     </row>
     <row r="35" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C35" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D35">
-        <v>1101</v>
+        <v>2111</v>
       </c>
       <c r="E35" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F35">
-        <v>1100</v>
+        <v>2110</v>
       </c>
     </row>
     <row r="36" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C36" t="s">
-        <v>26</v>
-      </c>
       <c r="D36">
-        <v>1111</v>
-      </c>
-      <c r="E36" t="s">
-        <v>26</v>
-      </c>
-      <c r="F36">
-        <v>1110</v>
+        <v>2112</v>
       </c>
     </row>
     <row r="38" spans="3:6" x14ac:dyDescent="0.3">
@@ -778,23 +797,23 @@
         <v>27</v>
       </c>
       <c r="D38">
-        <v>1201</v>
+        <v>2201</v>
       </c>
       <c r="E38" t="s">
         <v>27</v>
       </c>
       <c r="F38">
-        <v>1200</v>
+        <v>2200</v>
       </c>
     </row>
     <row r="39" spans="3:6" x14ac:dyDescent="0.3">
       <c r="D39">
-        <v>1202</v>
+        <v>2202</v>
       </c>
     </row>
     <row r="40" spans="3:6" x14ac:dyDescent="0.3">
       <c r="D40">
-        <v>1203</v>
+        <v>2203</v>
       </c>
     </row>
     <row r="41" spans="3:6" x14ac:dyDescent="0.3">
@@ -802,23 +821,23 @@
         <v>28</v>
       </c>
       <c r="D41">
-        <v>1211</v>
+        <v>2211</v>
       </c>
       <c r="E41" t="s">
         <v>28</v>
       </c>
       <c r="F41">
-        <v>1210</v>
+        <v>2210</v>
       </c>
     </row>
     <row r="42" spans="3:6" x14ac:dyDescent="0.3">
       <c r="D42">
-        <v>1212</v>
+        <v>2212</v>
       </c>
     </row>
     <row r="43" spans="3:6" x14ac:dyDescent="0.3">
       <c r="D43">
-        <v>1213</v>
+        <v>2213</v>
       </c>
     </row>
     <row r="45" spans="3:6" x14ac:dyDescent="0.3">
@@ -826,13 +845,13 @@
         <v>20</v>
       </c>
       <c r="D45">
-        <v>1301</v>
+        <v>2301</v>
       </c>
       <c r="E45" t="s">
         <v>20</v>
       </c>
       <c r="F45">
-        <v>1300</v>
+        <v>2300</v>
       </c>
     </row>
     <row r="46" spans="3:6" x14ac:dyDescent="0.3">
@@ -840,13 +859,13 @@
         <v>21</v>
       </c>
       <c r="D46">
-        <v>1311</v>
+        <v>2311</v>
       </c>
       <c r="E46" t="s">
         <v>21</v>
       </c>
       <c r="F46">
-        <v>1310</v>
+        <v>2310</v>
       </c>
     </row>
     <row r="48" spans="3:6" x14ac:dyDescent="0.3">
@@ -854,58 +873,58 @@
         <v>14</v>
       </c>
       <c r="D48">
-        <v>1401</v>
+        <v>2401</v>
       </c>
       <c r="E48" t="s">
         <v>14</v>
       </c>
       <c r="F48">
-        <v>1400</v>
-      </c>
-    </row>
-    <row r="49" spans="2:6" x14ac:dyDescent="0.3">
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C49" t="s">
         <v>15</v>
       </c>
       <c r="D49">
-        <v>1411</v>
+        <v>2411</v>
       </c>
       <c r="E49" t="s">
         <v>15</v>
       </c>
       <c r="F49">
-        <v>1410</v>
-      </c>
-    </row>
-    <row r="51" spans="2:6" x14ac:dyDescent="0.3">
+        <v>2410</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C51" t="s">
         <v>16</v>
       </c>
       <c r="D51">
-        <v>1501</v>
+        <v>2501</v>
       </c>
       <c r="E51" t="s">
         <v>16</v>
       </c>
       <c r="F51">
-        <v>1500</v>
-      </c>
-    </row>
-    <row r="52" spans="2:6" x14ac:dyDescent="0.3">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C52" t="s">
         <v>17</v>
       </c>
       <c r="D52">
-        <v>1511</v>
+        <v>2511</v>
       </c>
       <c r="E52" t="s">
         <v>17</v>
       </c>
       <c r="F52">
-        <v>1510</v>
-      </c>
-    </row>
-    <row r="55" spans="2:6" x14ac:dyDescent="0.3">
+        <v>2510</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B55" t="s">
         <v>22</v>
       </c>
@@ -913,16 +932,162 @@
         <v>22</v>
       </c>
       <c r="D55">
-        <v>2001</v>
+        <v>4001</v>
       </c>
       <c r="E55" t="s">
         <v>22</v>
       </c>
       <c r="F55">
-        <v>2000</v>
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>30</v>
+      </c>
+      <c r="B59" t="s">
+        <v>34</v>
+      </c>
+      <c r="C59" t="s">
+        <v>35</v>
+      </c>
+      <c r="D59">
+        <v>100001</v>
+      </c>
+      <c r="E59" t="s">
+        <v>34</v>
+      </c>
+      <c r="F59">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D60">
+        <v>100002</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B62" t="s">
+        <v>22</v>
+      </c>
+      <c r="C62" t="s">
+        <v>22</v>
+      </c>
+      <c r="D62">
+        <v>101001</v>
+      </c>
+      <c r="E62" t="s">
+        <v>22</v>
+      </c>
+      <c r="F62">
+        <v>101000</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2063A4A3-12ED-4192-9904-9108C69EF2EB}">
+  <dimension ref="A1:F12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C15" sqref="A15:C15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="6" width="15.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2">
+        <v>1000001</v>
+      </c>
+      <c r="E2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5">
+        <v>1010001</v>
+      </c>
+      <c r="E5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5">
+        <v>1010000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D6">
+        <v>1010002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D7">
+        <v>1010003</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10">
+        <v>1020001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D11">
+        <v>1020002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D12">
+        <v>1020003</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add id convention document
</commit_message>
<xml_diff>
--- a/IDSheet.xlsx
+++ b/IDSheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Learning\HK2Nam2\Introduction to Game Development\GameDev\GameMario\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC9706D5-69FE-49E3-BE28-836BAA08FC8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA523EF5-7BE9-456E-B45E-D24A318B91DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dynamic Object" sheetId="1" r:id="rId1"/>
@@ -462,8 +462,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A63" sqref="A63"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="R11" sqref="R11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
properly render question block
</commit_message>
<xml_diff>
--- a/IDSheet.xlsx
+++ b/IDSheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Learning\HK2Nam2\Introduction to Game Development\GameDev\GameMario\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA523EF5-7BE9-456E-B45E-D24A318B91DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{469DA171-8BA5-4119-B947-9831FD3B2887}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dynamic Object" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="40">
   <si>
     <t>Object</t>
   </si>
@@ -134,14 +134,34 @@
   </si>
   <si>
     <t xml:space="preserve">walk </t>
+  </si>
+  <si>
+    <t>question block</t>
+  </si>
+  <si>
+    <t>not hit</t>
+  </si>
+  <si>
+    <t>hit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hit </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -175,11 +195,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -462,7 +483,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F62"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="R11" sqref="R11"/>
     </sheetView>
   </sheetViews>
@@ -990,10 +1011,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2063A4A3-12ED-4192-9904-9108C69EF2EB}">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="A15:C15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1038,52 +1059,102 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>32</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C6" t="s">
         <v>32</v>
       </c>
-      <c r="D5">
+      <c r="D6">
         <v>1010001</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E6" t="s">
         <v>32</v>
       </c>
-      <c r="F5">
+      <c r="F6">
         <v>1010000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D6">
-        <v>1010002</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D7">
+        <v>1010002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D8">
         <v>1010003</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>33</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C12" t="s">
         <v>33</v>
       </c>
-      <c r="D10">
+      <c r="D12">
         <v>1020001</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D11">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D13">
         <v>1020002</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D12">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D14">
         <v>1020003</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="2"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" t="s">
+        <v>37</v>
+      </c>
+      <c r="D18">
+        <v>1030001</v>
+      </c>
+      <c r="E18" t="s">
+        <v>37</v>
+      </c>
+      <c r="F18">
+        <v>1030000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D19">
+        <v>1030002</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D20">
+        <v>1030003</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
+        <v>38</v>
+      </c>
+      <c r="C22" t="s">
+        <v>39</v>
+      </c>
+      <c r="D22">
+        <v>1031001</v>
+      </c>
+      <c r="E22" t="s">
+        <v>38</v>
+      </c>
+      <c r="F22">
+        <v>1031000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add mushroom object that move properly (perhaps)
</commit_message>
<xml_diff>
--- a/IDSheet.xlsx
+++ b/IDSheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Learning\HK2Nam2\Introduction to Game Development\GameDev\GameMario\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{469DA171-8BA5-4119-B947-9831FD3B2887}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD0717B9-BD05-455B-90C7-F13E03F877D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dynamic Object" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="41">
   <si>
     <t>Object</t>
   </si>
@@ -146,6 +146,9 @@
   </si>
   <si>
     <t xml:space="preserve">hit </t>
+  </si>
+  <si>
+    <t>mushroom</t>
   </si>
 </sst>
 </file>
@@ -481,10 +484,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F62"/>
+  <dimension ref="A1:F66"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="R11" sqref="R11"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F66" sqref="F66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1004,6 +1007,17 @@
         <v>101000</v>
       </c>
     </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>40</v>
+      </c>
+      <c r="D66">
+        <v>110001</v>
+      </c>
+      <c r="F66">
+        <v>110000</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1013,8 +1027,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2063A4A3-12ED-4192-9904-9108C69EF2EB}">
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F26" sqref="A26:F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
add edible mushroom and superleaf
</commit_message>
<xml_diff>
--- a/IDSheet.xlsx
+++ b/IDSheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Learning\HK2Nam2\Introduction to Game Development\GameDev\GameMario\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD0717B9-BD05-455B-90C7-F13E03F877D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FE47B68-983C-47B7-8D9B-891DB1BE9AC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dynamic Object" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="42">
   <si>
     <t>Object</t>
   </si>
@@ -136,9 +136,6 @@
     <t xml:space="preserve">walk </t>
   </si>
   <si>
-    <t>question block</t>
-  </si>
-  <si>
     <t>not hit</t>
   </si>
   <si>
@@ -149,6 +146,12 @@
   </si>
   <si>
     <t>mushroom</t>
+  </si>
+  <si>
+    <t>superleaf</t>
+  </si>
+  <si>
+    <t>questionblock</t>
   </si>
 </sst>
 </file>
@@ -484,10 +487,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F66"/>
+  <dimension ref="A1:F70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F66" sqref="F66"/>
+    <sheetView topLeftCell="A46" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1009,13 +1012,24 @@
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D66">
         <v>110001</v>
       </c>
       <c r="F66">
         <v>110000</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>40</v>
+      </c>
+      <c r="D70">
+        <v>120001</v>
+      </c>
+      <c r="F70">
+        <v>120000</v>
       </c>
     </row>
   </sheetData>
@@ -1027,8 +1041,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2063A4A3-12ED-4192-9904-9108C69EF2EB}">
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F26" sqref="A26:F26"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1126,19 +1140,19 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
+        <v>41</v>
+      </c>
+      <c r="B18" t="s">
         <v>36</v>
       </c>
-      <c r="B18" t="s">
-        <v>37</v>
-      </c>
       <c r="C18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D18">
         <v>1030001</v>
       </c>
       <c r="E18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F18">
         <v>1030000</v>
@@ -1156,16 +1170,16 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
+        <v>37</v>
+      </c>
+      <c r="C22" t="s">
         <v>38</v>
-      </c>
-      <c r="C22" t="s">
-        <v>39</v>
       </c>
       <c r="D22">
         <v>1031001</v>
       </c>
       <c r="E22" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F22">
         <v>1031000</v>

</xml_diff>

<commit_message>
Completed Box and Platform
</commit_message>
<xml_diff>
--- a/IDSheet.xlsx
+++ b/IDSheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Learning\HK2Nam2\Introduction to Game Development\GameDev\GameMario\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\source\repos\game-mario\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{469DA171-8BA5-4119-B947-9831FD3B2887}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5055B56-733A-40D4-A2B7-ED4D26A51F84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dynamic Object" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="61">
   <si>
     <t>Object</t>
   </si>
@@ -146,6 +146,69 @@
   </si>
   <si>
     <t xml:space="preserve">hit </t>
+  </si>
+  <si>
+    <t>box</t>
+  </si>
+  <si>
+    <t>orange</t>
+  </si>
+  <si>
+    <t>orange top left</t>
+  </si>
+  <si>
+    <t>orange top center</t>
+  </si>
+  <si>
+    <t>orange top right</t>
+  </si>
+  <si>
+    <t>orange middle left</t>
+  </si>
+  <si>
+    <t>orange middle center</t>
+  </si>
+  <si>
+    <t>orange middle right</t>
+  </si>
+  <si>
+    <t>orange bottom left</t>
+  </si>
+  <si>
+    <t>orange bottom center</t>
+  </si>
+  <si>
+    <t>orange bottom right</t>
+  </si>
+  <si>
+    <t>orange top shadow</t>
+  </si>
+  <si>
+    <t>orange middle shadow</t>
+  </si>
+  <si>
+    <t>orange bottom shadow</t>
+  </si>
+  <si>
+    <t>platform</t>
+  </si>
+  <si>
+    <t>top left</t>
+  </si>
+  <si>
+    <t>top center</t>
+  </si>
+  <si>
+    <t>top right</t>
+  </si>
+  <si>
+    <t>bottom left</t>
+  </si>
+  <si>
+    <t>bottom center</t>
+  </si>
+  <si>
+    <t>bottom right</t>
   </si>
 </sst>
 </file>
@@ -156,7 +219,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -164,7 +227,7 @@
       <i/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -487,12 +550,12 @@
       <selection activeCell="R11" sqref="R11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="6" width="15.77734375" customWidth="1"/>
+    <col min="1" max="6" width="15.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -512,7 +575,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -532,7 +595,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>8</v>
       </c>
@@ -546,7 +609,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>10</v>
       </c>
@@ -560,12 +623,12 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D6">
         <v>102</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>11</v>
       </c>
@@ -579,12 +642,12 @@
         <v>110</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D8">
         <v>112</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
         <v>12</v>
       </c>
@@ -598,17 +661,17 @@
         <v>200</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D11">
         <v>202</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D12">
         <v>203</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
         <v>13</v>
       </c>
@@ -622,17 +685,17 @@
         <v>210</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D14">
         <v>212</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D15">
         <v>213</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
         <v>14</v>
       </c>
@@ -646,7 +709,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
         <v>15</v>
       </c>
@@ -660,7 +723,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
         <v>16</v>
       </c>
@@ -674,7 +737,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
         <v>17</v>
       </c>
@@ -688,7 +751,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
         <v>19</v>
       </c>
@@ -702,7 +765,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
         <v>18</v>
       </c>
@@ -716,7 +779,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
         <v>20</v>
       </c>
@@ -730,7 +793,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
         <v>21</v>
       </c>
@@ -744,7 +807,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>23</v>
       </c>
@@ -761,7 +824,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C31" t="s">
         <v>24</v>
       </c>
@@ -775,7 +838,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="33" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C33" t="s">
         <v>25</v>
       </c>
@@ -789,12 +852,12 @@
         <v>2100</v>
       </c>
     </row>
-    <row r="34" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D34">
         <v>2102</v>
       </c>
     </row>
-    <row r="35" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C35" t="s">
         <v>26</v>
       </c>
@@ -808,12 +871,12 @@
         <v>2110</v>
       </c>
     </row>
-    <row r="36" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D36">
         <v>2112</v>
       </c>
     </row>
-    <row r="38" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C38" t="s">
         <v>27</v>
       </c>
@@ -827,17 +890,17 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="39" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D39">
         <v>2202</v>
       </c>
     </row>
-    <row r="40" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D40">
         <v>2203</v>
       </c>
     </row>
-    <row r="41" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C41" t="s">
         <v>28</v>
       </c>
@@ -851,17 +914,17 @@
         <v>2210</v>
       </c>
     </row>
-    <row r="42" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D42">
         <v>2212</v>
       </c>
     </row>
-    <row r="43" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D43">
         <v>2213</v>
       </c>
     </row>
-    <row r="45" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C45" t="s">
         <v>20</v>
       </c>
@@ -875,7 +938,7 @@
         <v>2300</v>
       </c>
     </row>
-    <row r="46" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C46" t="s">
         <v>21</v>
       </c>
@@ -889,7 +952,7 @@
         <v>2310</v>
       </c>
     </row>
-    <row r="48" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C48" t="s">
         <v>14</v>
       </c>
@@ -903,7 +966,7 @@
         <v>2400</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C49" t="s">
         <v>15</v>
       </c>
@@ -917,7 +980,7 @@
         <v>2410</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C51" t="s">
         <v>16</v>
       </c>
@@ -931,7 +994,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C52" t="s">
         <v>17</v>
       </c>
@@ -945,7 +1008,7 @@
         <v>2510</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
         <v>22</v>
       </c>
@@ -962,7 +1025,7 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>30</v>
       </c>
@@ -982,12 +1045,12 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D60">
         <v>100002</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
         <v>22</v>
       </c>
@@ -1011,18 +1074,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2063A4A3-12ED-4192-9904-9108C69EF2EB}">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40:D42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="6" width="15.77734375" customWidth="1"/>
+    <col min="1" max="6" width="15.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1042,7 +1105,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>31</v>
       </c>
@@ -1059,7 +1122,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>32</v>
       </c>
@@ -1076,17 +1139,17 @@
         <v>1010000</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D7">
         <v>1010002</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D8">
         <v>1010003</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>33</v>
       </c>
@@ -1097,20 +1160,20 @@
         <v>1020001</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D13">
         <v>1020002</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D14">
         <v>1020003</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A17" s="2"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>36</v>
       </c>
@@ -1130,17 +1193,17 @@
         <v>1030000</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D19">
         <v>1030002</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D20">
         <v>1030003</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>38</v>
       </c>
@@ -1155,6 +1218,159 @@
       </c>
       <c r="F22">
         <v>1031000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>40</v>
+      </c>
+      <c r="B24" t="s">
+        <v>41</v>
+      </c>
+      <c r="C24" t="s">
+        <v>42</v>
+      </c>
+      <c r="D24">
+        <v>1061001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
+        <v>43</v>
+      </c>
+      <c r="D25">
+        <v>1061002</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
+        <v>44</v>
+      </c>
+      <c r="D26">
+        <v>1061003</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
+        <v>45</v>
+      </c>
+      <c r="D27">
+        <v>1061004</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
+        <v>46</v>
+      </c>
+      <c r="D28">
+        <v>1061005</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
+        <v>47</v>
+      </c>
+      <c r="D29">
+        <v>1061006</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C30" t="s">
+        <v>48</v>
+      </c>
+      <c r="D30">
+        <v>1061007</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C31" t="s">
+        <v>49</v>
+      </c>
+      <c r="D31">
+        <v>1061008</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
+        <v>50</v>
+      </c>
+      <c r="D32">
+        <v>1061009</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C33" t="s">
+        <v>51</v>
+      </c>
+      <c r="D33">
+        <v>1061011</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C34" t="s">
+        <v>52</v>
+      </c>
+      <c r="D34">
+        <v>1061012</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C35" t="s">
+        <v>53</v>
+      </c>
+      <c r="D35">
+        <v>1061013</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>54</v>
+      </c>
+      <c r="C37" t="s">
+        <v>55</v>
+      </c>
+      <c r="D37">
+        <v>1071001</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C38" t="s">
+        <v>56</v>
+      </c>
+      <c r="D38">
+        <v>1071002</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C39" t="s">
+        <v>57</v>
+      </c>
+      <c r="D39">
+        <v>1071003</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C40" t="s">
+        <v>58</v>
+      </c>
+      <c r="D40">
+        <v>1072001</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C41" t="s">
+        <v>59</v>
+      </c>
+      <c r="D41">
+        <v>1072002</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C42" t="s">
+        <v>60</v>
+      </c>
+      <c r="D42">
+        <v>1072003</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
handle mushroom spawning, moving depends on collision direction properly
</commit_message>
<xml_diff>
--- a/IDSheet.xlsx
+++ b/IDSheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Learning\HK2Nam2\Introduction to Game Development\GameDev\GameMario\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FE47B68-983C-47B7-8D9B-891DB1BE9AC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A8664EB-8276-4C77-9B4B-0F36DEB9B461}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1752" yWindow="0" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dynamic Object" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="44">
   <si>
     <t>Object</t>
   </si>
@@ -152,6 +152,12 @@
   </si>
   <si>
     <t>questionblock</t>
+  </si>
+  <si>
+    <t>power up left</t>
+  </si>
+  <si>
+    <t>power up right</t>
   </si>
 </sst>
 </file>
@@ -487,10 +493,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F70"/>
+  <dimension ref="A1:F75"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B46" sqref="B46"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E53" sqref="E53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -951,84 +957,122 @@
         <v>2510</v>
       </c>
     </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C54" t="s">
+        <v>42</v>
+      </c>
+      <c r="D54">
+        <v>1</v>
+      </c>
+      <c r="E54" t="s">
+        <v>42</v>
+      </c>
+      <c r="F54">
+        <v>2600</v>
+      </c>
+    </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B55" t="s">
+      <c r="D55">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C56" t="s">
+        <v>43</v>
+      </c>
+      <c r="D56">
+        <v>11</v>
+      </c>
+      <c r="E56" t="s">
+        <v>43</v>
+      </c>
+      <c r="F56">
+        <v>2610</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D57">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B60" t="s">
         <v>22</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C60" t="s">
         <v>22</v>
       </c>
-      <c r="D55">
+      <c r="D60">
         <v>4001</v>
       </c>
-      <c r="E55" t="s">
+      <c r="E60" t="s">
         <v>22</v>
       </c>
-      <c r="F55">
+      <c r="F60">
         <v>4000</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A59" t="s">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
         <v>30</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B64" t="s">
         <v>34</v>
       </c>
-      <c r="C59" t="s">
+      <c r="C64" t="s">
         <v>35</v>
       </c>
-      <c r="D59">
+      <c r="D64">
         <v>100001</v>
       </c>
-      <c r="E59" t="s">
+      <c r="E64" t="s">
         <v>34</v>
       </c>
-      <c r="F59">
+      <c r="F64">
         <v>100000</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D60">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D65">
         <v>100002</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B62" t="s">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B67" t="s">
         <v>22</v>
       </c>
-      <c r="C62" t="s">
+      <c r="C67" t="s">
         <v>22</v>
       </c>
-      <c r="D62">
+      <c r="D67">
         <v>101001</v>
       </c>
-      <c r="E62" t="s">
+      <c r="E67" t="s">
         <v>22</v>
       </c>
-      <c r="F62">
+      <c r="F67">
         <v>101000</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A66" t="s">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
         <v>39</v>
       </c>
-      <c r="D66">
+      <c r="D71">
         <v>110001</v>
       </c>
-      <c r="F66">
+      <c r="F71">
         <v>110000</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A70" t="s">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
         <v>40</v>
       </c>
-      <c r="D70">
+      <c r="D75">
         <v>120001</v>
       </c>
-      <c r="F70">
+      <c r="F75">
         <v>120000</v>
       </c>
     </row>
@@ -1041,8 +1085,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2063A4A3-12ED-4192-9904-9108C69EF2EB}">
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
handle mario power up animation properly
</commit_message>
<xml_diff>
--- a/IDSheet.xlsx
+++ b/IDSheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Learning\HK2Nam2\Introduction to Game Development\GameDev\GameMario\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A8664EB-8276-4C77-9B4B-0F36DEB9B461}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D1779BD-93EA-419A-B5B6-ED8CC2AE4445}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1752" yWindow="0" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -495,8 +495,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E53" sqref="E53"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E57" sqref="E57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -973,7 +973,7 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D55">
-        <v>2001</v>
+        <v>2601</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
@@ -992,7 +992,7 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D57">
-        <v>2011</v>
+        <v>2611</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
buff objects remain buggy when stick near to each other
</commit_message>
<xml_diff>
--- a/IDSheet.xlsx
+++ b/IDSheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Learning\HK2Nam2\Introduction to Game Development\GameDev\GameMario\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D1779BD-93EA-419A-B5B6-ED8CC2AE4445}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCA37B4B-0A3D-4A18-938C-5D4C839C6CFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1752" yWindow="0" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -493,10 +493,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F75"/>
+  <dimension ref="A1:F76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E57" sqref="E57"/>
+    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G76" sqref="G76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1074,6 +1074,14 @@
       </c>
       <c r="F75">
         <v>120000</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D76">
+        <v>120011</v>
+      </c>
+      <c r="F76">
+        <v>120010</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Merged ID Track sheet
</commit_message>
<xml_diff>
--- a/IDSheet.xlsx
+++ b/IDSheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Learning\HK2Nam2\Introduction to Game Development\GameDev\GameMario\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\source\repos\game-mario\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCA37B4B-0A3D-4A18-938C-5D4C839C6CFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED42C62C-BC9B-4CDB-8AD1-3E735C1FC0D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1752" yWindow="0" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="9960" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dynamic Object" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="73">
   <si>
     <t>Object</t>
   </si>
@@ -151,13 +151,100 @@
     <t>superleaf</t>
   </si>
   <si>
-    <t>questionblock</t>
-  </si>
-  <si>
     <t>power up left</t>
   </si>
   <si>
     <t>power up right</t>
+  </si>
+  <si>
+    <t>top left</t>
+  </si>
+  <si>
+    <t>top center</t>
+  </si>
+  <si>
+    <t>top right</t>
+  </si>
+  <si>
+    <t>bottom left</t>
+  </si>
+  <si>
+    <t>bottom center</t>
+  </si>
+  <si>
+    <t>bottom right</t>
+  </si>
+  <si>
+    <t>question block</t>
+  </si>
+  <si>
+    <t>box</t>
+  </si>
+  <si>
+    <t>orange</t>
+  </si>
+  <si>
+    <t>orange top left</t>
+  </si>
+  <si>
+    <t>orange top center</t>
+  </si>
+  <si>
+    <t>orange top right</t>
+  </si>
+  <si>
+    <t>orange middle left</t>
+  </si>
+  <si>
+    <t>orange middle center</t>
+  </si>
+  <si>
+    <t>orange middle right</t>
+  </si>
+  <si>
+    <t>orange bottom left</t>
+  </si>
+  <si>
+    <t>orange bottom center</t>
+  </si>
+  <si>
+    <t>orange bottom right</t>
+  </si>
+  <si>
+    <t>top right shadow</t>
+  </si>
+  <si>
+    <t>middle right shadow</t>
+  </si>
+  <si>
+    <t>bottom left shadow</t>
+  </si>
+  <si>
+    <t>bottom center shadow</t>
+  </si>
+  <si>
+    <t>bottom right shadow</t>
+  </si>
+  <si>
+    <t>platform</t>
+  </si>
+  <si>
+    <t>tree</t>
+  </si>
+  <si>
+    <t>bottom without border</t>
+  </si>
+  <si>
+    <t>bottom left border</t>
+  </si>
+  <si>
+    <t>bottom right border</t>
+  </si>
+  <si>
+    <t>pipe</t>
+  </si>
+  <si>
+    <t>bush</t>
   </si>
 </sst>
 </file>
@@ -168,7 +255,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -176,7 +263,7 @@
       <i/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -495,16 +582,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G76" sqref="G76"/>
+    <sheetView topLeftCell="A27" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A81" sqref="A81:D133"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="6" width="15.77734375" customWidth="1"/>
+    <col min="1" max="6" width="15.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -524,7 +611,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -544,7 +631,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>8</v>
       </c>
@@ -558,7 +645,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>10</v>
       </c>
@@ -572,12 +659,12 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D6">
         <v>102</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>11</v>
       </c>
@@ -591,12 +678,12 @@
         <v>110</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D8">
         <v>112</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
         <v>12</v>
       </c>
@@ -610,17 +697,17 @@
         <v>200</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D11">
         <v>202</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D12">
         <v>203</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
         <v>13</v>
       </c>
@@ -634,17 +721,17 @@
         <v>210</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D14">
         <v>212</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D15">
         <v>213</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
         <v>14</v>
       </c>
@@ -658,7 +745,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
         <v>15</v>
       </c>
@@ -672,7 +759,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
         <v>16</v>
       </c>
@@ -686,7 +773,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
         <v>17</v>
       </c>
@@ -700,7 +787,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
         <v>19</v>
       </c>
@@ -714,7 +801,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
         <v>18</v>
       </c>
@@ -728,7 +815,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
         <v>20</v>
       </c>
@@ -742,7 +829,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
         <v>21</v>
       </c>
@@ -756,7 +843,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>23</v>
       </c>
@@ -773,7 +860,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C31" t="s">
         <v>24</v>
       </c>
@@ -787,7 +874,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="33" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C33" t="s">
         <v>25</v>
       </c>
@@ -801,12 +888,12 @@
         <v>2100</v>
       </c>
     </row>
-    <row r="34" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D34">
         <v>2102</v>
       </c>
     </row>
-    <row r="35" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C35" t="s">
         <v>26</v>
       </c>
@@ -820,12 +907,12 @@
         <v>2110</v>
       </c>
     </row>
-    <row r="36" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D36">
         <v>2112</v>
       </c>
     </row>
-    <row r="38" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C38" t="s">
         <v>27</v>
       </c>
@@ -839,17 +926,17 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="39" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D39">
         <v>2202</v>
       </c>
     </row>
-    <row r="40" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D40">
         <v>2203</v>
       </c>
     </row>
-    <row r="41" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C41" t="s">
         <v>28</v>
       </c>
@@ -863,17 +950,17 @@
         <v>2210</v>
       </c>
     </row>
-    <row r="42" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D42">
         <v>2212</v>
       </c>
     </row>
-    <row r="43" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D43">
         <v>2213</v>
       </c>
     </row>
-    <row r="45" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C45" t="s">
         <v>20</v>
       </c>
@@ -887,7 +974,7 @@
         <v>2300</v>
       </c>
     </row>
-    <row r="46" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C46" t="s">
         <v>21</v>
       </c>
@@ -901,7 +988,7 @@
         <v>2310</v>
       </c>
     </row>
-    <row r="48" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C48" t="s">
         <v>14</v>
       </c>
@@ -915,7 +1002,7 @@
         <v>2400</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C49" t="s">
         <v>15</v>
       </c>
@@ -929,7 +1016,7 @@
         <v>2410</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C51" t="s">
         <v>16</v>
       </c>
@@ -943,7 +1030,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C52" t="s">
         <v>17</v>
       </c>
@@ -957,45 +1044,45 @@
         <v>2510</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C54" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D54">
         <v>1</v>
       </c>
       <c r="E54" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F54">
         <v>2600</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D55">
         <v>2601</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C56" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D56">
         <v>11</v>
       </c>
       <c r="E56" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F56">
         <v>2610</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D57">
         <v>2611</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
         <v>22</v>
       </c>
@@ -1012,7 +1099,7 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>30</v>
       </c>
@@ -1032,12 +1119,12 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D65">
         <v>100002</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
         <v>22</v>
       </c>
@@ -1054,7 +1141,7 @@
         <v>101000</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>39</v>
       </c>
@@ -1065,7 +1152,7 @@
         <v>110000</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>40</v>
       </c>
@@ -1076,7 +1163,7 @@
         <v>120000</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D76">
         <v>120011</v>
       </c>
@@ -1091,18 +1178,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2063A4A3-12ED-4192-9904-9108C69EF2EB}">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:F64"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="6" width="15.77734375" customWidth="1"/>
+    <col min="1" max="6" width="15.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1122,7 +1209,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>31</v>
       </c>
@@ -1139,7 +1226,7 @@
         <v>1000000</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>32</v>
       </c>
@@ -1156,85 +1243,368 @@
         <v>1010000</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D7">
         <v>1010002</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D8">
         <v>1010003</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>33</v>
       </c>
       <c r="C12" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="D12">
-        <v>1020001</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+        <v>1020110</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>44</v>
+      </c>
       <c r="D13">
-        <v>1020002</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+        <v>1020120</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>45</v>
+      </c>
       <c r="D14">
-        <v>1020003</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+        <v>1020130</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>46</v>
+      </c>
+      <c r="D15">
+        <v>1020210</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>47</v>
+      </c>
+      <c r="D16">
+        <v>1020220</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A17" s="2"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>41</v>
-      </c>
-      <c r="B18" t="s">
+      <c r="C17" t="s">
+        <v>48</v>
+      </c>
+      <c r="D17">
+        <v>1020230</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>49</v>
+      </c>
+      <c r="B24" t="s">
         <v>36</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C24" t="s">
         <v>36</v>
       </c>
-      <c r="D18">
+      <c r="D24">
         <v>1030001</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E24" t="s">
         <v>36</v>
       </c>
-      <c r="F18">
+      <c r="F24">
         <v>1030000</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D19">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D25">
         <v>1030002</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D20">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D26">
         <v>1030003</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B22" t="s">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
         <v>37</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C28" t="s">
         <v>38</v>
       </c>
-      <c r="D22">
+      <c r="D28">
         <v>1031001</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E28" t="s">
         <v>37</v>
       </c>
-      <c r="F22">
+      <c r="F28">
         <v>1031000</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>50</v>
+      </c>
+      <c r="B30" t="s">
+        <v>51</v>
+      </c>
+      <c r="C30" t="s">
+        <v>52</v>
+      </c>
+      <c r="D30">
+        <v>1061110</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C31" t="s">
+        <v>53</v>
+      </c>
+      <c r="D31">
+        <v>1061120</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
+        <v>54</v>
+      </c>
+      <c r="D32">
+        <v>1061130</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C33" t="s">
+        <v>55</v>
+      </c>
+      <c r="D33">
+        <v>1061210</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C34" t="s">
+        <v>56</v>
+      </c>
+      <c r="D34">
+        <v>1061220</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C35" t="s">
+        <v>57</v>
+      </c>
+      <c r="D35">
+        <v>1061230</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C36" t="s">
+        <v>58</v>
+      </c>
+      <c r="D36">
+        <v>1061310</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C37" t="s">
+        <v>59</v>
+      </c>
+      <c r="D37">
+        <v>1061320</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C38" t="s">
+        <v>60</v>
+      </c>
+      <c r="D38">
+        <v>1061330</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C39" t="s">
+        <v>61</v>
+      </c>
+      <c r="D39">
+        <v>1060130</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C40" t="s">
+        <v>62</v>
+      </c>
+      <c r="D40">
+        <v>1060230</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C41" t="s">
+        <v>63</v>
+      </c>
+      <c r="D41">
+        <v>1060310</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C42" t="s">
+        <v>64</v>
+      </c>
+      <c r="D42">
+        <v>1060320</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C43" t="s">
+        <v>65</v>
+      </c>
+      <c r="D43">
+        <v>1060330</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>66</v>
+      </c>
+      <c r="C46" t="s">
+        <v>43</v>
+      </c>
+      <c r="D46">
+        <v>1070110</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C47" t="s">
+        <v>44</v>
+      </c>
+      <c r="D47">
+        <v>1070120</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C48" t="s">
+        <v>45</v>
+      </c>
+      <c r="D48">
+        <v>1070130</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C49" t="s">
+        <v>46</v>
+      </c>
+      <c r="D49">
+        <v>1070210</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C50" t="s">
+        <v>47</v>
+      </c>
+      <c r="D50">
+        <v>1070220</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C51" t="s">
+        <v>48</v>
+      </c>
+      <c r="D51">
+        <v>1070230</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>67</v>
+      </c>
+      <c r="C53" t="s">
+        <v>43</v>
+      </c>
+      <c r="D53">
+        <v>1080110</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C54" t="s">
+        <v>45</v>
+      </c>
+      <c r="D54">
+        <v>1080120</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C55" t="s">
+        <v>68</v>
+      </c>
+      <c r="D55">
+        <v>1080200</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C56" t="s">
+        <v>69</v>
+      </c>
+      <c r="D56">
+        <v>1080210</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C57" t="s">
+        <v>70</v>
+      </c>
+      <c r="D57">
+        <v>1080220</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>71</v>
+      </c>
+      <c r="C59" t="s">
+        <v>43</v>
+      </c>
+      <c r="D59">
+        <v>1090110</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C60" t="s">
+        <v>45</v>
+      </c>
+      <c r="D60">
+        <v>1090120</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C61" t="s">
+        <v>46</v>
+      </c>
+      <c r="D61">
+        <v>1090210</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C62" t="s">
+        <v>48</v>
+      </c>
+      <c r="D62">
+        <v>1090220</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>72</v>
+      </c>
+      <c r="D64">
+        <v>1100000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Drawn most of map 1-1
</commit_message>
<xml_diff>
--- a/IDSheet.xlsx
+++ b/IDSheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\source\repos\game-mario\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED42C62C-BC9B-4CDB-8AD1-3E735C1FC0D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C99ED3A8-7CDA-428F-A9F9-F0338DFDCB8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="9960" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4080" yWindow="2508" windowWidth="17280" windowHeight="9960" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dynamic Object" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="118">
   <si>
     <t>Object</t>
   </si>
@@ -245,6 +245,141 @@
   </si>
   <si>
     <t>bush</t>
+  </si>
+  <si>
+    <t>striped brick</t>
+  </si>
+  <si>
+    <t>trinket</t>
+  </si>
+  <si>
+    <t>flower</t>
+  </si>
+  <si>
+    <t>star</t>
+  </si>
+  <si>
+    <t>shadow</t>
+  </si>
+  <si>
+    <t>blue</t>
+  </si>
+  <si>
+    <t>blue top left</t>
+  </si>
+  <si>
+    <t>blue top center</t>
+  </si>
+  <si>
+    <t>blue top right</t>
+  </si>
+  <si>
+    <t>blue middle left</t>
+  </si>
+  <si>
+    <t>blue middle center</t>
+  </si>
+  <si>
+    <t>blue middle right</t>
+  </si>
+  <si>
+    <t>blue bottom left</t>
+  </si>
+  <si>
+    <t>blue bottom center</t>
+  </si>
+  <si>
+    <t>blue bottom right</t>
+  </si>
+  <si>
+    <t>green</t>
+  </si>
+  <si>
+    <t>green top left</t>
+  </si>
+  <si>
+    <t>green top center</t>
+  </si>
+  <si>
+    <t>green top right</t>
+  </si>
+  <si>
+    <t>green middle left</t>
+  </si>
+  <si>
+    <t>green middle center</t>
+  </si>
+  <si>
+    <t>green middle right</t>
+  </si>
+  <si>
+    <t>green bottom left</t>
+  </si>
+  <si>
+    <t>green bottom center</t>
+  </si>
+  <si>
+    <t>green bottom right</t>
+  </si>
+  <si>
+    <t>white</t>
+  </si>
+  <si>
+    <t>white top left</t>
+  </si>
+  <si>
+    <t>white top center</t>
+  </si>
+  <si>
+    <t>white top right</t>
+  </si>
+  <si>
+    <t>white middle left</t>
+  </si>
+  <si>
+    <t>white middle center</t>
+  </si>
+  <si>
+    <t>white middle right</t>
+  </si>
+  <si>
+    <t>black</t>
+  </si>
+  <si>
+    <t>black top left</t>
+  </si>
+  <si>
+    <t>black top center</t>
+  </si>
+  <si>
+    <t>black top right</t>
+  </si>
+  <si>
+    <t>black middle left</t>
+  </si>
+  <si>
+    <t>black middle center</t>
+  </si>
+  <si>
+    <t>black middle right</t>
+  </si>
+  <si>
+    <t>black bottom left</t>
+  </si>
+  <si>
+    <t>black bottom center</t>
+  </si>
+  <si>
+    <t>black bottom right</t>
+  </si>
+  <si>
+    <t>ending</t>
+  </si>
+  <si>
+    <t>ending transition</t>
+  </si>
+  <si>
+    <t>ending background</t>
   </si>
 </sst>
 </file>
@@ -582,7 +717,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F76"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A58" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="A81" sqref="A81:D133"/>
     </sheetView>
   </sheetViews>
@@ -1178,10 +1313,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2063A4A3-12ED-4192-9904-9108C69EF2EB}">
-  <dimension ref="A1:F64"/>
+  <dimension ref="A1:F107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1226,6 +1361,14 @@
         <v>1000000</v>
       </c>
     </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D3">
+        <v>1000002</v>
+      </c>
+    </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>32</v>
@@ -1357,254 +1500,579 @@
         <v>50</v>
       </c>
       <c r="B30" t="s">
-        <v>51</v>
+        <v>77</v>
       </c>
       <c r="C30" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="D30">
-        <v>1061110</v>
+        <v>1060130</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C31" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="D31">
-        <v>1061120</v>
+        <v>1060230</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C32" t="s">
+        <v>63</v>
+      </c>
+      <c r="D32">
+        <v>1060310</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C33" t="s">
+        <v>64</v>
+      </c>
+      <c r="D33">
+        <v>1060320</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C34" t="s">
+        <v>65</v>
+      </c>
+      <c r="D34">
+        <v>1060330</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>115</v>
+      </c>
+      <c r="C36" t="s">
+        <v>116</v>
+      </c>
+      <c r="D36">
+        <v>1060001</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C37" t="s">
+        <v>117</v>
+      </c>
+      <c r="D37">
+        <v>1060002</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>51</v>
+      </c>
+      <c r="C38" t="s">
+        <v>52</v>
+      </c>
+      <c r="D38">
+        <v>1061110</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C39" t="s">
+        <v>53</v>
+      </c>
+      <c r="D39">
+        <v>1061120</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C40" t="s">
         <v>54</v>
       </c>
-      <c r="D32">
+      <c r="D40">
         <v>1061130</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C33" t="s">
+    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C41" t="s">
         <v>55</v>
       </c>
-      <c r="D33">
+      <c r="D41">
         <v>1061210</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C34" t="s">
+    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C42" t="s">
         <v>56</v>
       </c>
-      <c r="D34">
+      <c r="D42">
         <v>1061220</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C35" t="s">
+    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C43" t="s">
         <v>57</v>
       </c>
-      <c r="D35">
+      <c r="D43">
         <v>1061230</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C36" t="s">
+    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C44" t="s">
         <v>58</v>
       </c>
-      <c r="D36">
+      <c r="D44">
         <v>1061310</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C37" t="s">
+    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C45" t="s">
         <v>59</v>
       </c>
-      <c r="D37">
+      <c r="D45">
         <v>1061320</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C38" t="s">
+    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C46" t="s">
         <v>60</v>
       </c>
-      <c r="D38">
+      <c r="D46">
         <v>1061330</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C39" t="s">
-        <v>61</v>
-      </c>
-      <c r="D39">
-        <v>1060130</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C40" t="s">
-        <v>62</v>
-      </c>
-      <c r="D40">
-        <v>1060230</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C41" t="s">
-        <v>63</v>
-      </c>
-      <c r="D41">
-        <v>1060310</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C42" t="s">
-        <v>64</v>
-      </c>
-      <c r="D42">
-        <v>1060320</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C43" t="s">
-        <v>65</v>
-      </c>
-      <c r="D43">
-        <v>1060330</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>78</v>
+      </c>
+      <c r="C48" t="s">
+        <v>79</v>
+      </c>
+      <c r="D48">
+        <v>1062110</v>
+      </c>
+    </row>
+    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C49" t="s">
+        <v>80</v>
+      </c>
+      <c r="D49">
+        <v>1062120</v>
+      </c>
+    </row>
+    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C50" t="s">
+        <v>81</v>
+      </c>
+      <c r="D50">
+        <v>1062130</v>
+      </c>
+    </row>
+    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C51" t="s">
+        <v>82</v>
+      </c>
+      <c r="D51">
+        <v>1062210</v>
+      </c>
+    </row>
+    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C52" t="s">
+        <v>83</v>
+      </c>
+      <c r="D52">
+        <v>1062220</v>
+      </c>
+    </row>
+    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C53" t="s">
+        <v>84</v>
+      </c>
+      <c r="D53">
+        <v>1062230</v>
+      </c>
+    </row>
+    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C54" t="s">
+        <v>85</v>
+      </c>
+      <c r="D54">
+        <v>1062310</v>
+      </c>
+    </row>
+    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C55" t="s">
+        <v>86</v>
+      </c>
+      <c r="D55">
+        <v>1062320</v>
+      </c>
+    </row>
+    <row r="56" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C56" t="s">
+        <v>87</v>
+      </c>
+      <c r="D56">
+        <v>1062330</v>
+      </c>
+    </row>
+    <row r="58" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
+        <v>88</v>
+      </c>
+      <c r="C58" t="s">
+        <v>89</v>
+      </c>
+      <c r="D58">
+        <v>1063110</v>
+      </c>
+    </row>
+    <row r="59" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C59" t="s">
+        <v>90</v>
+      </c>
+      <c r="D59">
+        <v>1063120</v>
+      </c>
+    </row>
+    <row r="60" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C60" t="s">
+        <v>91</v>
+      </c>
+      <c r="D60">
+        <v>1063130</v>
+      </c>
+    </row>
+    <row r="61" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C61" t="s">
+        <v>92</v>
+      </c>
+      <c r="D61">
+        <v>1063210</v>
+      </c>
+    </row>
+    <row r="62" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C62" t="s">
+        <v>93</v>
+      </c>
+      <c r="D62">
+        <v>1063220</v>
+      </c>
+    </row>
+    <row r="63" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C63" t="s">
+        <v>94</v>
+      </c>
+      <c r="D63">
+        <v>1063230</v>
+      </c>
+    </row>
+    <row r="64" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C64" t="s">
+        <v>95</v>
+      </c>
+      <c r="D64">
+        <v>1063310</v>
+      </c>
+    </row>
+    <row r="65" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C65" t="s">
+        <v>96</v>
+      </c>
+      <c r="D65">
+        <v>1063320</v>
+      </c>
+    </row>
+    <row r="66" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C66" t="s">
+        <v>97</v>
+      </c>
+      <c r="D66">
+        <v>1063330</v>
+      </c>
+    </row>
+    <row r="68" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B68" t="s">
+        <v>98</v>
+      </c>
+      <c r="C68" t="s">
+        <v>99</v>
+      </c>
+      <c r="D68">
+        <v>1064110</v>
+      </c>
+    </row>
+    <row r="69" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C69" t="s">
+        <v>100</v>
+      </c>
+      <c r="D69">
+        <v>1064120</v>
+      </c>
+    </row>
+    <row r="70" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C70" t="s">
+        <v>101</v>
+      </c>
+      <c r="D70">
+        <v>1064130</v>
+      </c>
+    </row>
+    <row r="71" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C71" t="s">
+        <v>102</v>
+      </c>
+      <c r="D71">
+        <v>1064210</v>
+      </c>
+    </row>
+    <row r="72" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C72" t="s">
+        <v>103</v>
+      </c>
+      <c r="D72">
+        <v>1064220</v>
+      </c>
+    </row>
+    <row r="73" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C73" t="s">
+        <v>104</v>
+      </c>
+      <c r="D73">
+        <v>1064230</v>
+      </c>
+    </row>
+    <row r="75" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B75" t="s">
+        <v>105</v>
+      </c>
+      <c r="C75" t="s">
+        <v>106</v>
+      </c>
+      <c r="D75">
+        <v>1065110</v>
+      </c>
+    </row>
+    <row r="76" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C76" t="s">
+        <v>107</v>
+      </c>
+      <c r="D76">
+        <v>1065120</v>
+      </c>
+    </row>
+    <row r="77" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C77" t="s">
+        <v>108</v>
+      </c>
+      <c r="D77">
+        <v>1065130</v>
+      </c>
+    </row>
+    <row r="78" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C78" t="s">
+        <v>109</v>
+      </c>
+      <c r="D78">
+        <v>1065210</v>
+      </c>
+    </row>
+    <row r="79" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C79" t="s">
+        <v>110</v>
+      </c>
+      <c r="D79">
+        <v>1065220</v>
+      </c>
+    </row>
+    <row r="80" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C80" t="s">
+        <v>111</v>
+      </c>
+      <c r="D80">
+        <v>1065230</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C81" t="s">
+        <v>112</v>
+      </c>
+      <c r="D81">
+        <v>1065310</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C82" t="s">
+        <v>113</v>
+      </c>
+      <c r="D82">
+        <v>1065320</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C83" t="s">
+        <v>114</v>
+      </c>
+      <c r="D83">
+        <v>1065330</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
         <v>66</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C85" t="s">
         <v>43</v>
       </c>
-      <c r="D46">
+      <c r="D85">
         <v>1070110</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C47" t="s">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C86" t="s">
         <v>44</v>
       </c>
-      <c r="D47">
+      <c r="D86">
         <v>1070120</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C48" t="s">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C87" t="s">
         <v>45</v>
       </c>
-      <c r="D48">
+      <c r="D87">
         <v>1070130</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C49" t="s">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C88" t="s">
         <v>46</v>
       </c>
-      <c r="D49">
+      <c r="D88">
         <v>1070210</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C50" t="s">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C89" t="s">
         <v>47</v>
       </c>
-      <c r="D50">
+      <c r="D89">
         <v>1070220</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C51" t="s">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C90" t="s">
         <v>48</v>
       </c>
-      <c r="D51">
+      <c r="D90">
         <v>1070230</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
         <v>67</v>
       </c>
-      <c r="C53" t="s">
+      <c r="C92" t="s">
         <v>43</v>
       </c>
-      <c r="D53">
+      <c r="D92">
         <v>1080110</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C54" t="s">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C93" t="s">
         <v>45</v>
       </c>
-      <c r="D54">
+      <c r="D93">
         <v>1080120</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C55" t="s">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C94" t="s">
         <v>68</v>
       </c>
-      <c r="D55">
+      <c r="D94">
         <v>1080200</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C56" t="s">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C95" t="s">
         <v>69</v>
       </c>
-      <c r="D56">
+      <c r="D95">
         <v>1080210</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C57" t="s">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C96" t="s">
         <v>70</v>
       </c>
-      <c r="D57">
+      <c r="D96">
         <v>1080220</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
         <v>71</v>
       </c>
-      <c r="C59" t="s">
+      <c r="C98" t="s">
         <v>43</v>
       </c>
-      <c r="D59">
+      <c r="D98">
         <v>1090110</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C60" t="s">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C99" t="s">
         <v>45</v>
       </c>
-      <c r="D60">
+      <c r="D99">
         <v>1090120</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C61" t="s">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C100" t="s">
         <v>46</v>
       </c>
-      <c r="D61">
+      <c r="D100">
         <v>1090210</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C62" t="s">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C101" t="s">
         <v>48</v>
       </c>
-      <c r="D62">
+      <c r="D101">
         <v>1090220</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
         <v>72</v>
       </c>
-      <c r="D64">
+      <c r="D103">
         <v>1100000</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>74</v>
+      </c>
+      <c r="C105" t="s">
+        <v>75</v>
+      </c>
+      <c r="D105">
+        <v>1110001</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C106" t="s">
+        <v>76</v>
+      </c>
+      <c r="D106">
+        <v>1110002</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C107" t="s">
+        <v>39</v>
+      </c>
+      <c r="D107">
+        <v>1110003</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Piranha Plant (no shooting mechanism)
</commit_message>
<xml_diff>
--- a/IDSheet.xlsx
+++ b/IDSheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\source\repos\game-mario\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1A0D38A-5D50-4FDD-AD32-17A6F3E01261}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EE24494-0CD6-429E-B5E7-5B394547C573}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4080" yWindow="2508" windowWidth="17280" windowHeight="9960" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4080" yWindow="2508" windowWidth="17280" windowHeight="9960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dynamic Object" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="135">
   <si>
     <t>Object</t>
   </si>
@@ -380,6 +380,57 @@
   </si>
   <si>
     <t>ending background</t>
+  </si>
+  <si>
+    <t>piranha plant</t>
+  </si>
+  <si>
+    <t>top left closed</t>
+  </si>
+  <si>
+    <t>top left opened</t>
+  </si>
+  <si>
+    <t>bottom left closed</t>
+  </si>
+  <si>
+    <t>bottom left opened</t>
+  </si>
+  <si>
+    <t>top right closed</t>
+  </si>
+  <si>
+    <t>top right opened</t>
+  </si>
+  <si>
+    <t>bottom right closed</t>
+  </si>
+  <si>
+    <t>bottom right opened</t>
+  </si>
+  <si>
+    <t>upright closed</t>
+  </si>
+  <si>
+    <t>upright opened</t>
+  </si>
+  <si>
+    <t>top left shoot</t>
+  </si>
+  <si>
+    <t>bottom left shoot</t>
+  </si>
+  <si>
+    <t>bottom right shoot</t>
+  </si>
+  <si>
+    <t>top right shoot</t>
+  </si>
+  <si>
+    <t>left move</t>
+  </si>
+  <si>
+    <t>right move</t>
   </si>
 </sst>
 </file>
@@ -715,10 +766,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F76"/>
+  <dimension ref="A1:F87"/>
   <sheetViews>
-    <sheetView topLeftCell="A58" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A81" sqref="A81:D133"/>
+    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E81" sqref="E81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1306,6 +1357,125 @@
         <v>120010</v>
       </c>
     </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>118</v>
+      </c>
+      <c r="C78" t="s">
+        <v>119</v>
+      </c>
+      <c r="D78">
+        <v>130110</v>
+      </c>
+      <c r="E78" t="s">
+        <v>133</v>
+      </c>
+      <c r="F78">
+        <v>130000</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C79" t="s">
+        <v>120</v>
+      </c>
+      <c r="D79">
+        <v>130111</v>
+      </c>
+      <c r="E79" t="s">
+        <v>129</v>
+      </c>
+      <c r="F79">
+        <v>130110</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C80" t="s">
+        <v>121</v>
+      </c>
+      <c r="D80">
+        <v>130210</v>
+      </c>
+      <c r="E80" t="s">
+        <v>130</v>
+      </c>
+      <c r="F80">
+        <v>130210</v>
+      </c>
+    </row>
+    <row r="81" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C81" t="s">
+        <v>122</v>
+      </c>
+      <c r="D81">
+        <v>130211</v>
+      </c>
+    </row>
+    <row r="82" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C82" t="s">
+        <v>123</v>
+      </c>
+      <c r="D82">
+        <v>130120</v>
+      </c>
+      <c r="E82" t="s">
+        <v>134</v>
+      </c>
+      <c r="F82">
+        <v>130010</v>
+      </c>
+    </row>
+    <row r="83" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C83" t="s">
+        <v>124</v>
+      </c>
+      <c r="D83">
+        <v>130121</v>
+      </c>
+      <c r="E83" t="s">
+        <v>132</v>
+      </c>
+      <c r="F83">
+        <v>130120</v>
+      </c>
+    </row>
+    <row r="84" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C84" t="s">
+        <v>125</v>
+      </c>
+      <c r="D84">
+        <v>130220</v>
+      </c>
+      <c r="E84" t="s">
+        <v>131</v>
+      </c>
+      <c r="F84">
+        <v>130220</v>
+      </c>
+    </row>
+    <row r="85" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C85" t="s">
+        <v>126</v>
+      </c>
+      <c r="D85">
+        <v>130221</v>
+      </c>
+    </row>
+    <row r="86" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C86" t="s">
+        <v>127</v>
+      </c>
+      <c r="D86">
+        <v>130000</v>
+      </c>
+    </row>
+    <row r="87" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C87" t="s">
+        <v>128</v>
+      </c>
+      <c r="D87">
+        <v>130001</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1315,7 +1485,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2063A4A3-12ED-4192-9904-9108C69EF2EB}">
   <dimension ref="A1:F108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
+    <sheetView topLeftCell="A80" workbookViewId="0">
       <selection activeCell="D91" sqref="D91"/>
     </sheetView>
   </sheetViews>

</xml_diff>